<commit_message>
(feat) stock automation ready
(feat) stock automation ready
</commit_message>
<xml_diff>
--- a/ExempleTD/TecDoc.xlsx
+++ b/ExempleTD/TecDoc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://renovatioautomotive.sharepoint.com/sites/IT1/Documents partages/Ebay_shop/Product/Exemple avec le second template/ExempleTD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlotte\Github\Automatisation-imports-fournisseurs\ExempleTD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="11_F25DC773A252ABDACC1048AF89DB6AE85ADE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A4EADA6-B1A0-450B-963D-D2720F710018}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB6779B-EDD5-4970-B360-867400198F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="401" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-8310" windowWidth="51840" windowHeight="21120" tabRatio="401" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Marque</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>5500 N</t>
+  </si>
+  <si>
+    <t>111757,222222,333333,444444</t>
   </si>
 </sst>
 </file>
@@ -441,7 +444,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -502,8 +505,8 @@
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3">
-        <v>111757</v>
+      <c r="C2" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>17</v>
@@ -617,15 +620,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B220343EAFB5854FBFF7FA41F36ED3FC" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="73e61d5c86ed7c415c7e2679a037a901">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="234b9710-e223-44ab-9cc3-e21623e75daa" xmlns:ns3="882ee881-f9b4-4c15-8d7b-82171bd71b1f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8e56453268a23dfd6a317ae22eadfc92" ns2:_="" ns3:_="">
     <xsd:import namespace="234b9710-e223-44ab-9cc3-e21623e75daa"/>
@@ -836,6 +830,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -848,14 +851,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16C9DA40-2995-4053-9615-7F5DAAAF74D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7DC6DFF-4A0B-4B66-83D6-0F0C1A2E79FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -874,6 +869,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16C9DA40-2995-4053-9615-7F5DAAAF74D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AA2FFE5-8D3B-4DA2-A79F-6FB6E9881FEC}">
   <ds:schemaRefs>

</xml_diff>